<commit_message>
added comments and updated featuredNewsPage
</commit_message>
<xml_diff>
--- a/src/test/resources/newsData.xlsx
+++ b/src/test/resources/newsData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="20">
   <si>
     <t>Top 10 takeaways from our Q4 2023 earnings</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>All Apps &amp; Tools</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Cognizant shines at the Times Group Global Business Summit (GBS)</t>
   </si>
 </sst>
 </file>
@@ -512,7 +518,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s" s="3">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>12</v>

</xml_diff>